<commit_message>
V00.00.10.14 - Corrected bug with coarse control not going to fine control when because sp was compared with sensor offset
</commit_message>
<xml_diff>
--- a/Python/Controller Debug Variables.xlsx
+++ b/Python/Controller Debug Variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212596572\Documents\Projects\Github\PV624_MAIN\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DF4F66-3D36-438F-B972-3E079DAC742F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D535380-3995-43B6-B75F-0A14E2ABC9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CBE23F72-E2F0-4EB5-B2FB-CCEA5583A90C}"/>
   </bookViews>
@@ -1022,10 +1022,10 @@
     <t>reserved8</t>
   </si>
   <si>
-    <t>sensorGuageUncertainty</t>
-  </si>
-  <si>
-    <t>sensor['gaugeUncertainty']</t>
+    <t>sensorOffset</t>
+  </si>
+  <si>
+    <t>sensor['offset']</t>
   </si>
 </sst>
 </file>
@@ -1421,7 +1421,7 @@
   <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
V00.22.33 - Added dwell actions for fine control and controlled vent and associated bug fixes
</commit_message>
<xml_diff>
--- a/Python/Controller Debug Variables.xlsx
+++ b/Python/Controller Debug Variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212596572\Documents\Projects\Github\PV624_MAIN\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D535380-3995-43B6-B75F-0A14E2ABC9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F01A1DE-D37E-4662-910D-A712FBD556F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CBE23F72-E2F0-4EB5-B2FB-CCEA5583A90C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="333">
   <si>
     <t>Expression</t>
   </si>
@@ -83,9 +83,6 @@
     <t>pressureBaro</t>
   </si>
   <si>
-    <t>pressureOld</t>
-  </si>
-  <si>
     <t>stepSize</t>
   </si>
   <si>
@@ -251,12 +248,6 @@
     <t>ventDutyCycle</t>
   </si>
   <si>
-    <t>totalVentTime</t>
-  </si>
-  <si>
-    <t>dwellCount</t>
-  </si>
-  <si>
     <t>Header 1</t>
   </si>
   <si>
@@ -443,9 +434,6 @@
     <t>PID['baroP']</t>
   </si>
   <si>
-    <t>PID['oldPressureG']</t>
-  </si>
-  <si>
     <t>previous</t>
   </si>
   <si>
@@ -1026,6 +1014,27 @@
   </si>
   <si>
     <t>sensor['offset']</t>
+  </si>
+  <si>
+    <t>overshootDisabled</t>
+  </si>
+  <si>
+    <t>PID['overshootDisabled]</t>
+  </si>
+  <si>
+    <t>cvRequiredPressureReads</t>
+  </si>
+  <si>
+    <t>cvPressureReadCounter</t>
+  </si>
+  <si>
+    <t>cvChangeInPressure</t>
+  </si>
+  <si>
+    <t>oscillationDetected</t>
+  </si>
+  <si>
+    <t>pauseCycles</t>
   </si>
 </sst>
 </file>
@@ -1418,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0E5AEF4-3396-4D4E-B759-4B764B106E51}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1446,25 +1455,25 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F1">
-        <f>SUM(E2:E75)</f>
-        <v>296</v>
+        <f>SUM(E2:E78)</f>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -1472,16 +1481,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -1492,7 +1501,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1506,7 +1515,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1520,7 +1529,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1534,7 +1543,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1548,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -1562,7 +1571,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1576,7 +1585,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1590,7 +1599,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1604,7 +1613,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -1617,11 +1626,11 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>135</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -1631,11 +1640,11 @@
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>139</v>
+      <c r="B14" s="5" t="s">
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -1645,11 +1654,11 @@
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>140</v>
+      <c r="B15" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -1659,11 +1668,11 @@
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>143</v>
+      <c r="B16" t="s">
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -1674,10 +1683,10 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1685,13 +1694,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" t="s">
         <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -1699,13 +1708,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>326</v>
       </c>
       <c r="B19" t="s">
-        <v>148</v>
+        <v>327</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1713,13 +1722,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -1727,10 +1736,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -1741,10 +1750,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>156</v>
+        <v>328</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -1755,13 +1761,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>157</v>
+        <v>329</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E23">
         <v>4</v>
@@ -1769,13 +1772,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>164</v>
+        <v>330</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -1783,13 +1783,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>166</v>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>152</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E25">
         <v>4</v>
@@ -1797,10 +1797,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -1811,10 +1811,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>316</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1839,10 +1839,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -1853,10 +1853,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -1867,10 +1867,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>188</v>
+        <v>312</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -1881,10 +1881,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -1895,13 +1895,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -1909,10 +1909,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>202</v>
+        <v>32</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>184</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -1923,10 +1923,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
@@ -1937,13 +1937,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" t="s">
-        <v>208</v>
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E36">
         <v>4</v>
@@ -1951,10 +1951,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -1965,10 +1965,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
@@ -1979,10 +1979,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>215</v>
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>204</v>
       </c>
       <c r="C39" t="s">
         <v>6</v>
@@ -1993,10 +1993,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
@@ -2007,10 +2007,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>314</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
@@ -2021,10 +2021,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>231</v>
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -2035,10 +2035,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
@@ -2049,10 +2049,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>310</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="C44" t="s">
         <v>6</v>
@@ -2063,10 +2063,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>238</v>
+        <v>42</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>227</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -2077,10 +2077,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
@@ -2091,10 +2091,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
@@ -2105,10 +2105,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" t="s">
-        <v>247</v>
+        <v>45</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
@@ -2119,10 +2119,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" t="s">
-        <v>251</v>
+        <v>46</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="C49" t="s">
         <v>6</v>
@@ -2133,10 +2133,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
@@ -2147,10 +2147,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C51" t="s">
         <v>6</v>
@@ -2161,10 +2161,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>257</v>
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>247</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
@@ -2175,10 +2175,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>254</v>
+        <v>50</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
@@ -2189,10 +2189,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -2203,10 +2203,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" t="s">
-        <v>260</v>
+        <v>52</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
@@ -2217,13 +2217,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>261</v>
+        <v>53</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E56">
         <v>4</v>
@@ -2231,13 +2231,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>266</v>
+        <v>54</v>
+      </c>
+      <c r="B57" t="s">
+        <v>254</v>
       </c>
       <c r="C57" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E57">
         <v>4</v>
@@ -2245,13 +2245,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>271</v>
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>256</v>
       </c>
       <c r="C58" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E58">
         <v>4</v>
@@ -2259,13 +2259,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E59">
         <v>4</v>
@@ -2273,13 +2273,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" t="s">
-        <v>273</v>
+        <v>57</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E60">
         <v>4</v>
@@ -2287,13 +2287,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E61">
         <v>4</v>
@@ -2301,10 +2301,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" t="s">
-        <v>280</v>
+        <v>59</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
@@ -2315,10 +2315,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>285</v>
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>269</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
@@ -2329,10 +2329,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
@@ -2343,13 +2343,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>289</v>
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>276</v>
       </c>
       <c r="C65" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E65">
         <v>4</v>
@@ -2357,13 +2357,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>67</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>292</v>
+        <v>63</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="C66" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E66">
         <v>4</v>
@@ -2371,10 +2371,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
@@ -2385,13 +2385,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E68">
         <v>4</v>
@@ -2399,10 +2399,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C69" t="s">
         <v>4</v>
@@ -2413,13 +2413,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>71</v>
-      </c>
-      <c r="B70" t="s">
-        <v>304</v>
+        <v>67</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="C70" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E70">
         <v>4</v>
@@ -2427,13 +2427,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>72</v>
-      </c>
-      <c r="B71" t="s">
-        <v>310</v>
+        <v>68</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="C71" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E71">
         <v>4</v>
@@ -2441,13 +2441,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>328</v>
-      </c>
-      <c r="B72" t="s">
-        <v>329</v>
+        <v>69</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>294</v>
       </c>
       <c r="C72" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E72">
         <v>4</v>
@@ -2455,11 +2455,9 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>315</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>319</v>
-      </c>
+        <v>331</v>
+      </c>
+      <c r="B73" s="4"/>
       <c r="C73" t="s">
         <v>4</v>
       </c>
@@ -2469,13 +2467,11 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="B74" s="4"/>
       <c r="C74" t="s">
         <v>4</v>
-      </c>
-      <c r="D74" t="s">
-        <v>78</v>
       </c>
       <c r="E74">
         <v>4</v>
@@ -2483,15 +2479,57 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>324</v>
+      </c>
+      <c r="B75" t="s">
+        <v>325</v>
       </c>
       <c r="C75" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="E75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>311</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>73</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>75</v>
+      </c>
+      <c r="E77">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>74</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>75</v>
+      </c>
+      <c r="E78">
         <v>4</v>
       </c>
     </row>
@@ -2516,1900 +2554,1900 @@
   <sheetData>
     <row r="1" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H1">
         <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L1" t="s">
+        <v>156</v>
+      </c>
+      <c r="M1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N1" t="s">
         <v>158</v>
       </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
         <v>159</v>
-      </c>
-      <c r="L1" t="s">
-        <v>160</v>
-      </c>
-      <c r="M1" t="s">
-        <v>161</v>
-      </c>
-      <c r="N1" t="s">
-        <v>162</v>
-      </c>
-      <c r="O1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="2" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H2">
         <v>100</v>
       </c>
       <c r="I2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O2" t="s">
         <v>159</v>
-      </c>
-      <c r="L2" t="s">
-        <v>160</v>
-      </c>
-      <c r="M2" t="s">
-        <v>161</v>
-      </c>
-      <c r="N2" t="s">
-        <v>162</v>
-      </c>
-      <c r="O2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="3" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H4">
         <v>0.2</v>
       </c>
       <c r="I4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
+        <v>161</v>
+      </c>
+      <c r="K4" t="s">
+        <v>129</v>
+      </c>
+      <c r="L4" t="s">
+        <v>158</v>
+      </c>
+      <c r="M4" t="s">
+        <v>119</v>
+      </c>
+      <c r="N4" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P4" t="s">
         <v>165</v>
       </c>
-      <c r="K4" t="s">
-        <v>132</v>
-      </c>
-      <c r="L4" t="s">
-        <v>162</v>
-      </c>
-      <c r="M4" t="s">
-        <v>122</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>167</v>
       </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
+        <v>127</v>
+      </c>
+      <c r="S4" t="s">
+        <v>149</v>
+      </c>
+      <c r="T4" t="s">
         <v>168</v>
-      </c>
-      <c r="P4" t="s">
-        <v>169</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>171</v>
-      </c>
-      <c r="R4" t="s">
-        <v>130</v>
-      </c>
-      <c r="S4" t="s">
-        <v>153</v>
-      </c>
-      <c r="T4" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="5" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F5" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H5">
         <v>1000</v>
       </c>
       <c r="I5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J5" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H6">
         <v>1000</v>
       </c>
       <c r="I6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J6" t="s">
+        <v>172</v>
+      </c>
+      <c r="K6" t="s">
+        <v>173</v>
+      </c>
+      <c r="L6" t="s">
+        <v>174</v>
+      </c>
+      <c r="M6" t="s">
+        <v>140</v>
+      </c>
+      <c r="N6" t="s">
+        <v>125</v>
+      </c>
+      <c r="O6" t="s">
+        <v>111</v>
+      </c>
+      <c r="P6" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q6" t="s">
         <v>176</v>
       </c>
-      <c r="K6" t="s">
+      <c r="R6" t="s">
         <v>177</v>
       </c>
-      <c r="L6" t="s">
+      <c r="S6" t="s">
         <v>178</v>
       </c>
-      <c r="M6" t="s">
-        <v>144</v>
-      </c>
-      <c r="N6" t="s">
-        <v>128</v>
-      </c>
-      <c r="O6" t="s">
-        <v>114</v>
-      </c>
-      <c r="P6" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>180</v>
-      </c>
-      <c r="R6" t="s">
-        <v>181</v>
-      </c>
-      <c r="S6" t="s">
-        <v>182</v>
-      </c>
       <c r="T6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J7" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="L7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="M7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="N7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="P7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="Q7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="L8" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="M8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="K9" t="s">
+        <v>181</v>
+      </c>
+      <c r="L9" t="s">
+        <v>183</v>
+      </c>
+      <c r="M9" t="s">
+        <v>116</v>
+      </c>
+      <c r="N9" t="s">
+        <v>132</v>
+      </c>
+      <c r="O9" t="s">
+        <v>150</v>
+      </c>
+      <c r="P9" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>109</v>
+      </c>
+      <c r="R9" t="s">
         <v>185</v>
       </c>
-      <c r="L9" t="s">
-        <v>187</v>
-      </c>
-      <c r="M9" t="s">
-        <v>119</v>
-      </c>
-      <c r="N9" t="s">
-        <v>136</v>
-      </c>
-      <c r="O9" t="s">
-        <v>154</v>
-      </c>
-      <c r="P9" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>112</v>
-      </c>
-      <c r="R9" t="s">
-        <v>189</v>
-      </c>
       <c r="S9" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
+        <v>187</v>
+      </c>
+      <c r="G10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" t="s">
+        <v>160</v>
+      </c>
+      <c r="I10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10" t="s">
+        <v>157</v>
+      </c>
+      <c r="K10" t="s">
+        <v>119</v>
+      </c>
+      <c r="L10" t="s">
+        <v>156</v>
+      </c>
+      <c r="M10" t="s">
+        <v>188</v>
+      </c>
+      <c r="N10" t="s">
+        <v>189</v>
+      </c>
+      <c r="O10" t="s">
+        <v>134</v>
+      </c>
+      <c r="P10" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>134</v>
+      </c>
+      <c r="R10" t="s">
         <v>191</v>
       </c>
-      <c r="G10" t="s">
-        <v>109</v>
-      </c>
-      <c r="H10" t="s">
-        <v>164</v>
-      </c>
-      <c r="I10" t="s">
-        <v>110</v>
-      </c>
-      <c r="J10" t="s">
-        <v>161</v>
-      </c>
-      <c r="K10" t="s">
-        <v>122</v>
-      </c>
-      <c r="L10" t="s">
-        <v>160</v>
-      </c>
-      <c r="M10" t="s">
+      <c r="S10" t="s">
         <v>192</v>
       </c>
-      <c r="N10" t="s">
+      <c r="T10" t="s">
         <v>193</v>
       </c>
-      <c r="O10" t="s">
-        <v>138</v>
-      </c>
-      <c r="P10" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>138</v>
-      </c>
-      <c r="R10" t="s">
-        <v>195</v>
-      </c>
-      <c r="S10" t="s">
-        <v>196</v>
-      </c>
-      <c r="T10" t="s">
-        <v>197</v>
-      </c>
       <c r="U10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="V10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="W10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="M11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="N11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="K12" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="L12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M12" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="N12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="O12" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="P12" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J13" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K13" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="L13" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="M13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="N13" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O13" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="P13" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="Q13" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J14" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="K14" t="s">
+        <v>181</v>
+      </c>
+      <c r="L14" t="s">
+        <v>201</v>
+      </c>
+      <c r="M14" t="s">
+        <v>205</v>
+      </c>
+      <c r="N14" t="s">
+        <v>116</v>
+      </c>
+      <c r="O14" t="s">
+        <v>132</v>
+      </c>
+      <c r="P14" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>188</v>
+      </c>
+      <c r="R14" t="s">
+        <v>109</v>
+      </c>
+      <c r="S14" t="s">
         <v>185</v>
       </c>
-      <c r="L14" t="s">
-        <v>205</v>
-      </c>
-      <c r="M14" t="s">
-        <v>209</v>
-      </c>
-      <c r="N14" t="s">
-        <v>119</v>
-      </c>
-      <c r="O14" t="s">
-        <v>136</v>
-      </c>
-      <c r="P14" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>192</v>
-      </c>
-      <c r="R14" t="s">
-        <v>112</v>
-      </c>
-      <c r="S14" t="s">
-        <v>189</v>
-      </c>
       <c r="T14" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="K15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="M15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="N15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="O15" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H16" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J16" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K16" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="L16" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M16" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="O16" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="Q16" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G17" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H17" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J17" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K17" t="s">
+        <v>164</v>
+      </c>
+      <c r="L17" t="s">
+        <v>165</v>
+      </c>
+      <c r="M17" t="s">
+        <v>207</v>
+      </c>
+      <c r="N17" t="s">
+        <v>208</v>
+      </c>
+      <c r="O17" t="s">
+        <v>202</v>
+      </c>
+      <c r="P17" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>149</v>
+      </c>
+      <c r="R17" t="s">
         <v>168</v>
-      </c>
-      <c r="L17" t="s">
-        <v>169</v>
-      </c>
-      <c r="M17" t="s">
-        <v>211</v>
-      </c>
-      <c r="N17" t="s">
-        <v>212</v>
-      </c>
-      <c r="O17" t="s">
-        <v>206</v>
-      </c>
-      <c r="P17" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>153</v>
-      </c>
-      <c r="R17" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="18" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G18" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H18">
         <v>500</v>
       </c>
       <c r="I18" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J18" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K18" t="s">
+        <v>213</v>
+      </c>
+      <c r="L18" t="s">
+        <v>214</v>
+      </c>
+      <c r="M18" t="s">
+        <v>149</v>
+      </c>
+      <c r="N18" t="s">
+        <v>215</v>
+      </c>
+      <c r="O18" t="s">
+        <v>216</v>
+      </c>
+      <c r="P18" t="s">
         <v>217</v>
       </c>
-      <c r="L18" t="s">
+      <c r="Q18" t="s">
         <v>218</v>
       </c>
-      <c r="M18" t="s">
-        <v>153</v>
-      </c>
-      <c r="N18" t="s">
-        <v>219</v>
-      </c>
-      <c r="O18" t="s">
-        <v>220</v>
-      </c>
-      <c r="P18" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>222</v>
-      </c>
       <c r="R18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="S18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="I19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J19" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H20">
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J20" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="K20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L20" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M20" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="N20" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="O20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="P20" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="Q20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F21" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H21" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="I21" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J21" s="1">
         <v>1000000</v>
       </c>
       <c r="K21" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L21" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="M21" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="N21" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="O21" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="P21" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G22" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H22" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="I22" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J22" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="K22" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="L22">
         <v>2</v>
       </c>
       <c r="M22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N22" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="O22" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="P22" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="Q22" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F23" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G23" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H23" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="I23" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J23" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="K23" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="L23">
         <v>2</v>
       </c>
       <c r="M23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N23" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="O23" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="P23" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="Q23" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G24" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H24" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="I24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J24" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="K24" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="L24" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M24" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O24" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="P24" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F25" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H25" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="I25" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K25" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L25" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M25" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="N25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="O25" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="P25" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="Q25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="R25" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F26" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H26">
         <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J26" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K26" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="L26" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="M26" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="N26" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="O26" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="P26" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="Q26" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H27">
         <v>0.1</v>
       </c>
       <c r="I27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J27" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="K27" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="L27" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M27" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F28" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J28" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K28" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N28" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="O28" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F29" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="G29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J29" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K29" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="L29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M29" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="N29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="P29" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="G30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J30" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M30" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K31" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="L31" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N31" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="O31" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="6:19" x14ac:dyDescent="0.25">
       <c r="F32" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="G32" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H32">
         <v>0.98</v>
       </c>
       <c r="I32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J32" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="K32" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="L32" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="M32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="N32" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="O32" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="P32" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="Q32" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="R32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="G33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J33" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="K33" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M33" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="N33" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O33" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="P33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G34" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J34" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="K34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M34" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="N34" t="s">
+        <v>109</v>
+      </c>
+      <c r="O34" t="s">
+        <v>156</v>
+      </c>
+      <c r="P34" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>259</v>
+      </c>
+      <c r="R34" t="s">
+        <v>260</v>
+      </c>
+      <c r="S34" t="s">
         <v>112</v>
-      </c>
-      <c r="O34" t="s">
-        <v>160</v>
-      </c>
-      <c r="P34" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>263</v>
-      </c>
-      <c r="R34" t="s">
-        <v>264</v>
-      </c>
-      <c r="S34" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="35" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H35">
         <v>300</v>
       </c>
       <c r="I35" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J35" t="s">
+        <v>161</v>
+      </c>
+      <c r="K35" t="s">
+        <v>263</v>
+      </c>
+      <c r="L35" t="s">
+        <v>109</v>
+      </c>
+      <c r="M35" t="s">
+        <v>164</v>
+      </c>
+      <c r="N35" t="s">
         <v>165</v>
       </c>
-      <c r="K35" t="s">
-        <v>267</v>
-      </c>
-      <c r="L35" t="s">
-        <v>112</v>
-      </c>
-      <c r="M35" t="s">
-        <v>168</v>
-      </c>
-      <c r="N35" t="s">
-        <v>169</v>
-      </c>
       <c r="O35" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="P35" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q35" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="R35" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="S35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="T35" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F36" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="G36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H36">
         <v>10</v>
       </c>
       <c r="I36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J36" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="K36" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="L36" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M36" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="N36" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="O36" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="P36" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="Q36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="R36" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="S36" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="T36" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F37" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="G37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J37" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="K37" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="L37" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="M37" t="s">
+        <v>164</v>
+      </c>
+      <c r="N37" t="s">
+        <v>165</v>
+      </c>
+      <c r="O37" t="s">
+        <v>109</v>
+      </c>
+      <c r="P37" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>137</v>
+      </c>
+      <c r="R37" t="s">
+        <v>203</v>
+      </c>
+      <c r="S37" t="s">
+        <v>126</v>
+      </c>
+      <c r="T37" t="s">
+        <v>149</v>
+      </c>
+      <c r="U37" t="s">
         <v>168</v>
-      </c>
-      <c r="N37" t="s">
-        <v>169</v>
-      </c>
-      <c r="O37" t="s">
-        <v>112</v>
-      </c>
-      <c r="P37" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>141</v>
-      </c>
-      <c r="R37" t="s">
-        <v>207</v>
-      </c>
-      <c r="S37" t="s">
-        <v>129</v>
-      </c>
-      <c r="T37" t="s">
-        <v>153</v>
-      </c>
-      <c r="U37" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="38" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H38">
         <v>0.1</v>
       </c>
       <c r="I38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J38" t="s">
+        <v>270</v>
+      </c>
+      <c r="K38" t="s">
+        <v>271</v>
+      </c>
+      <c r="L38" t="s">
+        <v>265</v>
+      </c>
+      <c r="M38" t="s">
+        <v>272</v>
+      </c>
+      <c r="N38" t="s">
+        <v>146</v>
+      </c>
+      <c r="O38" t="s">
+        <v>109</v>
+      </c>
+      <c r="P38" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>137</v>
+      </c>
+      <c r="R38" t="s">
+        <v>203</v>
+      </c>
+      <c r="S38" t="s">
+        <v>273</v>
+      </c>
+      <c r="T38" t="s">
+        <v>134</v>
+      </c>
+      <c r="U38" t="s">
         <v>274</v>
-      </c>
-      <c r="K38" t="s">
-        <v>275</v>
-      </c>
-      <c r="L38" t="s">
-        <v>269</v>
-      </c>
-      <c r="M38" t="s">
-        <v>276</v>
-      </c>
-      <c r="N38" t="s">
-        <v>150</v>
-      </c>
-      <c r="O38" t="s">
-        <v>112</v>
-      </c>
-      <c r="P38" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>141</v>
-      </c>
-      <c r="R38" t="s">
-        <v>207</v>
-      </c>
-      <c r="S38" t="s">
-        <v>277</v>
-      </c>
-      <c r="T38" t="s">
-        <v>138</v>
-      </c>
-      <c r="U38" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="39" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F39" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G39" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J39" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M39" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="N39" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="O39" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="P39" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="Q39" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F40" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="G40" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H40">
         <v>-0.7</v>
       </c>
       <c r="I40" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J40" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K40" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="L40" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="M40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N40" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="O40" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="P40" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="Q40" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="R40" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="S40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="G41" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J41" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K41" t="s">
+        <v>278</v>
+      </c>
+      <c r="L41" t="s">
+        <v>164</v>
+      </c>
+      <c r="M41" t="s">
+        <v>165</v>
+      </c>
+      <c r="N41" t="s">
+        <v>116</v>
+      </c>
+      <c r="O41" t="s">
         <v>282</v>
       </c>
-      <c r="L41" t="s">
+      <c r="P41" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>122</v>
+      </c>
+      <c r="R41" t="s">
+        <v>126</v>
+      </c>
+      <c r="S41" t="s">
+        <v>149</v>
+      </c>
+      <c r="T41" t="s">
         <v>168</v>
-      </c>
-      <c r="M41" t="s">
-        <v>169</v>
-      </c>
-      <c r="N41" t="s">
-        <v>119</v>
-      </c>
-      <c r="O41" t="s">
-        <v>286</v>
-      </c>
-      <c r="P41" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>125</v>
-      </c>
-      <c r="R41" t="s">
-        <v>129</v>
-      </c>
-      <c r="S41" t="s">
-        <v>153</v>
-      </c>
-      <c r="T41" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="42" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G42" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J42" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="K42" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L42" t="b">
         <v>1</v>
       </c>
       <c r="M42" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="N42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="O42" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="P42" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G43" t="s">
+        <v>106</v>
+      </c>
+      <c r="H43" t="s">
+        <v>267</v>
+      </c>
+      <c r="I43" t="s">
+        <v>107</v>
+      </c>
+      <c r="J43" t="s">
+        <v>118</v>
+      </c>
+      <c r="K43" t="s">
+        <v>119</v>
+      </c>
+      <c r="L43" t="s">
+        <v>78</v>
+      </c>
+      <c r="M43" t="s">
+        <v>263</v>
+      </c>
+      <c r="N43" t="s">
+        <v>134</v>
+      </c>
+      <c r="O43" t="s">
+        <v>286</v>
+      </c>
+      <c r="P43" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q43" t="s">
         <v>109</v>
       </c>
-      <c r="H43" t="s">
-        <v>271</v>
-      </c>
-      <c r="I43" t="s">
-        <v>110</v>
-      </c>
-      <c r="J43" t="s">
-        <v>121</v>
-      </c>
-      <c r="K43" t="s">
-        <v>122</v>
-      </c>
-      <c r="L43" t="s">
-        <v>81</v>
-      </c>
-      <c r="M43" t="s">
-        <v>267</v>
-      </c>
-      <c r="N43" t="s">
-        <v>138</v>
-      </c>
-      <c r="O43" t="s">
-        <v>290</v>
-      </c>
-      <c r="P43" t="s">
-        <v>291</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>112</v>
-      </c>
       <c r="R43" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="S43" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="T43" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="U43" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="V43" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G44" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J44" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K44" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L44" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M44" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="N44" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O44" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="P44" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="Q44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="R44" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="G45" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J45" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="K45" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L45" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="M45" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="N45" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O45" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="P45" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="Q45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R45" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="G46" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J46" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="K46" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="L46" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="M46" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="N46" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O46" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="P46" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="Q46" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="R46" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
+        <v>294</v>
+      </c>
+      <c r="G47" t="s">
+        <v>106</v>
+      </c>
+      <c r="H47" t="s">
+        <v>295</v>
+      </c>
+      <c r="I47" t="s">
+        <v>107</v>
+      </c>
+      <c r="J47" t="s">
+        <v>296</v>
+      </c>
+      <c r="K47" t="s">
+        <v>108</v>
+      </c>
+      <c r="L47" t="s">
+        <v>119</v>
+      </c>
+      <c r="M47" t="s">
+        <v>148</v>
+      </c>
+      <c r="N47" t="s">
+        <v>297</v>
+      </c>
+      <c r="O47" t="s">
         <v>298</v>
       </c>
-      <c r="G47" t="s">
-        <v>109</v>
-      </c>
-      <c r="H47" t="s">
+      <c r="P47" t="s">
         <v>299</v>
-      </c>
-      <c r="I47" t="s">
-        <v>110</v>
-      </c>
-      <c r="J47" t="s">
-        <v>300</v>
-      </c>
-      <c r="K47" t="s">
-        <v>111</v>
-      </c>
-      <c r="L47" t="s">
-        <v>122</v>
-      </c>
-      <c r="M47" t="s">
-        <v>152</v>
-      </c>
-      <c r="N47" t="s">
-        <v>301</v>
-      </c>
-      <c r="O47" t="s">
-        <v>302</v>
-      </c>
-      <c r="P47" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="48" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G48" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J48" t="s">
+        <v>301</v>
+      </c>
+      <c r="K48" t="s">
+        <v>108</v>
+      </c>
+      <c r="L48" t="s">
+        <v>302</v>
+      </c>
+      <c r="M48" t="s">
+        <v>148</v>
+      </c>
+      <c r="N48" t="s">
+        <v>297</v>
+      </c>
+      <c r="O48" t="s">
+        <v>303</v>
+      </c>
+      <c r="P48" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>296</v>
+      </c>
+      <c r="R48" t="s">
         <v>305</v>
       </c>
-      <c r="K48" t="s">
-        <v>111</v>
-      </c>
-      <c r="L48" t="s">
-        <v>306</v>
-      </c>
-      <c r="M48" t="s">
-        <v>152</v>
-      </c>
-      <c r="N48" t="s">
-        <v>301</v>
-      </c>
-      <c r="O48" t="s">
-        <v>307</v>
-      </c>
-      <c r="P48" t="s">
-        <v>308</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>300</v>
-      </c>
-      <c r="R48" t="s">
-        <v>309</v>
-      </c>
       <c r="S48" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="T48" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="U48" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="49" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="G49" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H49">
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J49" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K49" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L49" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M49" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="N49" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="O49" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="P49" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="Q49" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="R49" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="S49" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="T49" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="U49" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4432,21 +4470,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -4462,7 +4500,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -4478,7 +4516,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -4494,7 +4532,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -4510,7 +4548,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -4526,7 +4564,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -4542,7 +4580,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -4558,7 +4596,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -4574,7 +4612,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -4590,7 +4628,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -4606,7 +4644,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -4622,7 +4660,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -4638,7 +4676,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B14">
         <v>12</v>
@@ -4654,7 +4692,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B15">
         <v>13</v>
@@ -4670,7 +4708,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B16">
         <v>14</v>
@@ -4686,7 +4724,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B17">
         <v>15</v>
@@ -4702,7 +4740,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B18">
         <v>16</v>
@@ -4718,7 +4756,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B19">
         <v>17</v>
@@ -4734,7 +4772,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B20">
         <v>18</v>
@@ -4750,7 +4788,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B21">
         <v>19</v>
@@ -4766,7 +4804,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B22">
         <v>20</v>
@@ -4782,7 +4820,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B23">
         <v>21</v>
@@ -4798,7 +4836,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B24">
         <v>22</v>
@@ -4814,7 +4852,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B25">
         <v>23</v>
@@ -4830,7 +4868,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B26" s="6">
         <v>24</v>
@@ -4846,7 +4884,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B27" s="6">
         <v>25</v>
@@ -4862,7 +4900,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B28" s="6">
         <v>26</v>
@@ -4878,7 +4916,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B29" s="6">
         <v>27</v>
@@ -4894,7 +4932,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B30" s="6">
         <v>28</v>
@@ -4910,7 +4948,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B31" s="6">
         <v>29</v>
@@ -4926,7 +4964,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B32" s="6">
         <v>30</v>
@@ -4942,7 +4980,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B33" s="6">
         <v>31</v>

</xml_diff>